<commit_message>
giving permissions for tables to students
</commit_message>
<xml_diff>
--- a/xlsx/DATA_TEMPLATESNEW.xlsx
+++ b/xlsx/DATA_TEMPLATESNEW.xlsx
@@ -5,6 +5,7 @@
   <sheets>
     <sheet name="mtech" sheetId="1" r:id="rId1"/>
     <sheet name="5.2.1" sheetId="2" r:id="rId2"/>
+    <sheet name="btech" sheetId="3" r:id="rId3"/>
   </sheets>
 </workbook>
 </file>
@@ -1048,4 +1049,355 @@
     <ignoredError numberStoredAsText="1" sqref="A1:N4"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:BC2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>University_RollNumber</v>
+      </c>
+      <c r="B1" t="str">
+        <v>First_Name</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Last_Name</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Gender</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Nationality</v>
+      </c>
+      <c r="F1" t="str">
+        <v>DOB</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Phone_Number</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Email_ID</v>
+      </c>
+      <c r="I1" t="str">
+        <v>ADHAR_Number</v>
+      </c>
+      <c r="J1" t="str">
+        <v>Address</v>
+      </c>
+      <c r="K1" t="str">
+        <v>District</v>
+      </c>
+      <c r="L1" t="str">
+        <v>State</v>
+      </c>
+      <c r="M1" t="str">
+        <v>Country</v>
+      </c>
+      <c r="N1" t="str">
+        <v>Pin_Code</v>
+      </c>
+      <c r="O1" t="str">
+        <v>Category</v>
+      </c>
+      <c r="P1" t="str">
+        <v>Sub_Category</v>
+      </c>
+      <c r="Q1" t="str">
+        <v>_10th_CGPA</v>
+      </c>
+      <c r="R1" t="str">
+        <v>_10th_Board</v>
+      </c>
+      <c r="S1" t="str">
+        <v>_10th_YOP</v>
+      </c>
+      <c r="T1" t="str">
+        <v>_12th_Percentage</v>
+      </c>
+      <c r="U1" t="str">
+        <v>_12th_Board</v>
+      </c>
+      <c r="V1" t="str">
+        <v>_12th_YOP</v>
+      </c>
+      <c r="W1" t="str">
+        <v>Diploma_Percentage</v>
+      </c>
+      <c r="X1" t="str">
+        <v>Diploma_Board</v>
+      </c>
+      <c r="Y1" t="str">
+        <v>Diploma_YOP</v>
+      </c>
+      <c r="Z1" t="str">
+        <v>Course_RegularORIntegrated</v>
+      </c>
+      <c r="AA1" t="str">
+        <v>Branch</v>
+      </c>
+      <c r="AB1" t="str">
+        <v>College_Name</v>
+      </c>
+      <c r="AC1" t="str">
+        <v>Course_CGPA</v>
+      </c>
+      <c r="AD1" t="str">
+        <v>Number_Of_Backlogs</v>
+      </c>
+      <c r="AE1" t="str">
+        <v>Entrance_Exam</v>
+      </c>
+      <c r="AF1" t="str">
+        <v>CET_Rank</v>
+      </c>
+      <c r="AG1" t="str">
+        <v>Course_YOP</v>
+      </c>
+      <c r="AH1" t="str">
+        <v>Certificate_Course</v>
+      </c>
+      <c r="AI1" t="str">
+        <v>Certificate_IssuedBy</v>
+      </c>
+      <c r="AJ1" t="str">
+        <v>CertificateUpload</v>
+      </c>
+      <c r="AK1" t="str">
+        <v>Program_name</v>
+      </c>
+      <c r="AL1" t="str">
+        <v>Program_code</v>
+      </c>
+      <c r="AM1" t="str">
+        <v>InternUpload</v>
+      </c>
+      <c r="AN1" t="str">
+        <v>CertificatePlatform</v>
+      </c>
+      <c r="AO1" t="str">
+        <v>StudyingYear</v>
+      </c>
+      <c r="AP1" t="str">
+        <v>Year</v>
+      </c>
+      <c r="AQ1" t="str">
+        <v>Name_of_the_Teacher</v>
+      </c>
+      <c r="AR1" t="str">
+        <v>Contact_Details</v>
+      </c>
+      <c r="AS1" t="str">
+        <v>Program_graduated_from</v>
+      </c>
+      <c r="AT1" t="str">
+        <v>Name_of_company</v>
+      </c>
+      <c r="AU1" t="str">
+        <v>Name_of_employer_with_contact_details</v>
+      </c>
+      <c r="AV1" t="str">
+        <v>Pay_Package_at_appointment</v>
+      </c>
+      <c r="AW1" t="str">
+        <v>NameOfTeacher</v>
+      </c>
+      <c r="AX1" t="str">
+        <v>Name_Of_Students</v>
+      </c>
+      <c r="AY1" t="str">
+        <v>Name_Of_Institution_joined</v>
+      </c>
+      <c r="AZ1" t="str">
+        <v>Name_Of_Programme_Admitted_To</v>
+      </c>
+      <c r="BA1" t="str">
+        <v>Upload</v>
+      </c>
+      <c r="BB1" t="str">
+        <v>list_of_students_undertaking</v>
+      </c>
+      <c r="BC1" t="str">
+        <v>Program_Graduated</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>421206421015</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Jaya</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Madhuri</v>
+      </c>
+      <c r="D2" t="str">
+        <v>female</v>
+      </c>
+      <c r="E2" t="str">
+        <v>Indian</v>
+      </c>
+      <c r="F2" t="str">
+        <v>1-23-2001</v>
+      </c>
+      <c r="G2" t="str">
+        <v>891987</v>
+      </c>
+      <c r="H2" t="str">
+        <v>421206421015@andhrauniversity.edu.in</v>
+      </c>
+      <c r="I2" t="str">
+        <v>9630798</v>
+      </c>
+      <c r="J2" t="str">
+        <v>14/205-A</v>
+      </c>
+      <c r="K2" t="str">
+        <v>Krishna</v>
+      </c>
+      <c r="L2" t="str">
+        <v>AP</v>
+      </c>
+      <c r="M2" t="str">
+        <v>India</v>
+      </c>
+      <c r="N2" t="str">
+        <v>521301</v>
+      </c>
+      <c r="O2" t="str">
+        <v>BC-B</v>
+      </c>
+      <c r="P2" t="str">
+        <v>padmasali</v>
+      </c>
+      <c r="Q2" t="str">
+        <v>9</v>
+      </c>
+      <c r="R2" t="str">
+        <v>ssc</v>
+      </c>
+      <c r="S2">
+        <v>2016</v>
+      </c>
+      <c r="T2" t="str">
+        <v>98</v>
+      </c>
+      <c r="U2" t="str">
+        <v>IPE</v>
+      </c>
+      <c r="V2">
+        <v>2018</v>
+      </c>
+      <c r="W2" t="str">
+        <v/>
+      </c>
+      <c r="X2" t="str">
+        <v/>
+      </c>
+      <c r="Y2" t="str">
+        <v/>
+      </c>
+      <c r="Z2" t="str">
+        <v>Regular</v>
+      </c>
+      <c r="AA2" t="str">
+        <v>CSE</v>
+      </c>
+      <c r="AB2" t="str">
+        <v>AUCE</v>
+      </c>
+      <c r="AC2" t="str">
+        <v>9</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2" t="str">
+        <v>AUCET</v>
+      </c>
+      <c r="AF2">
+        <v>1872</v>
+      </c>
+      <c r="AG2">
+        <v>2022</v>
+      </c>
+      <c r="AH2" t="str">
+        <v/>
+      </c>
+      <c r="AI2" t="str">
+        <v/>
+      </c>
+      <c r="AJ2" t="str">
+        <f>HYPERLINK("CertificateUpload_1688981249563.pdf")</f>
+        <v>CertificateUpload_1688981249563.pdf</v>
+      </c>
+      <c r="AK2" t="str">
+        <v>kjh</v>
+      </c>
+      <c r="AL2" t="str">
+        <v>kjh</v>
+      </c>
+      <c r="AM2" t="str">
+        <f>HYPERLINK("InternUpload_1688981249627.pdf")</f>
+        <v>InternUpload_1688981249627.pdf</v>
+      </c>
+      <c r="AN2" t="str">
+        <v/>
+      </c>
+      <c r="AO2" t="str">
+        <v>firstyear</v>
+      </c>
+      <c r="AP2" t="str">
+        <v>2019</v>
+      </c>
+      <c r="AQ2" t="str">
+        <v>jaya</v>
+      </c>
+      <c r="AR2" t="str">
+        <v>madhuri,89129</v>
+      </c>
+      <c r="AS2" t="str">
+        <v>andhrauniversity</v>
+      </c>
+      <c r="AT2" t="str">
+        <v>nucluesteq raipur</v>
+      </c>
+      <c r="AU2" t="str">
+        <v>supriya</v>
+      </c>
+      <c r="AV2" t="str">
+        <v>76</v>
+      </c>
+      <c r="AW2" t="str">
+        <v>jhb</v>
+      </c>
+      <c r="AX2" t="str">
+        <v>j</v>
+      </c>
+      <c r="AY2" t="str">
+        <v/>
+      </c>
+      <c r="AZ2" t="str">
+        <v/>
+      </c>
+      <c r="BA2" t="str">
+        <f>HYPERLINK("Upload_1689317571425.pdf")</f>
+        <v>Upload_1689317571425.pdf</v>
+      </c>
+      <c r="BB2" t="str">
+        <v/>
+      </c>
+      <c r="BC2" t="str">
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:BC2"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>